<commit_message>
fix: (upload-service) upload/download tags
</commit_message>
<xml_diff>
--- a/upload.xlsx
+++ b/upload.xlsx
@@ -6,14 +6,36 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="notes" r:id="rId3" sheetId="1"/>
-    <sheet name="ENGLISH" r:id="rId4" sheetId="2"/>
+    <sheet name="tags" r:id="rId3" sheetId="1"/>
+    <sheet name="notes" r:id="rId4" sheetId="2"/>
+    <sheet name="ENGLISH" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="379">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>essentialism</t>
+  </si>
+  <si>
+    <t>discipline</t>
+  </si>
+  <si>
+    <t>mindset</t>
+  </si>
+  <si>
+    <t>science</t>
+  </si>
+  <si>
+    <t>sport</t>
+  </si>
+  <si>
+    <t>competition</t>
+  </si>
   <si>
     <t>content</t>
   </si>
@@ -24,292 +46,280 @@
     <t>last seen at</t>
   </si>
   <si>
+    <t>What do I want to go big on?</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.044</t>
+  </si>
+  <si>
+    <t>The faintest pencil is better than the strongest memory</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.05</t>
+  </si>
+  <si>
+    <t>A little nonsense now and then is cherished by the wisest men</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.055</t>
+  </si>
+  <si>
+    <t>Your health is your greatest wealth</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.061</t>
+  </si>
+  <si>
+    <t>Escape to quiet thinking and boredom</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.067</t>
+  </si>
+  <si>
+    <t>Ultimate focus. Eliminate distractions</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.074</t>
+  </si>
+  <si>
+    <t>Exceptional people are built in solitude</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.08</t>
+  </si>
+  <si>
+    <t>The magic is that there is no magic. Start where you are. Don't stop</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.087</t>
+  </si>
+  <si>
+    <t>Not lack of time, but lack of direction</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.093</t>
+  </si>
+  <si>
+    <t>Be humble, stay hungry</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.1</t>
+  </si>
+  <si>
+    <t>Saying what you mean and meaning what you say</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.108</t>
+  </si>
+  <si>
+    <t>If it isn't a clear yes, then it's a clear no</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.119</t>
+  </si>
+  <si>
+    <t>To follow, without halt, one aim: there is the secret to success</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.127</t>
+  </si>
+  <si>
+    <t>Half of the troubles of this life can be traced to saying yes too quickly and not saying no soon enough</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.135</t>
+  </si>
+  <si>
+    <t>Less but better</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.144</t>
+  </si>
+  <si>
+    <t>The main thing is to keep the main thing the main thing</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.151</t>
+  </si>
+  <si>
+    <t>Comfortable with cutting losses</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.159</t>
+  </si>
+  <si>
+    <t>Stop making casual commitments</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.166</t>
+  </si>
+  <si>
+    <t>Pause before you speak</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.174</t>
+  </si>
+  <si>
+    <t>Get over the fear of missing out</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.181</t>
+  </si>
+  <si>
+    <t>I saw the angel in the marble and carved until I set him free</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.189</t>
+  </si>
+  <si>
+    <t>No is a complete sentence</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.197</t>
+  </si>
+  <si>
+    <t>If you don't set boundaries - there won't be any</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.204</t>
+  </si>
+  <si>
+    <t>Give me 6 hours to chop down a tree and I will spend the first 4 sharpening the axe</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.212</t>
+  </si>
+  <si>
+    <t>The only thing we can expect (with any great certainty) is the unexpected</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.22</t>
+  </si>
+  <si>
+    <t>To attain knowledge add things every day. To attain wisdom subtract things every day</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.228</t>
+  </si>
+  <si>
+    <t>All it takes is a small shove, then momentum will naturally build</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.241</t>
+  </si>
+  <si>
+    <t>Look for small changes you can do in areas you do often. There is power in steadiness and repetition</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.255</t>
+  </si>
+  <si>
+    <t>Done is better than perfect</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.266</t>
+  </si>
+  <si>
+    <t>Routine, in an intelligent man, is a sign of ambition</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.279</t>
+  </si>
+  <si>
+    <t>Routine eliminates nonessential distractions and enshrines the essentials</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.29</t>
+  </si>
+  <si>
+    <t>Do the most difficult thing first</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.302</t>
+  </si>
+  <si>
+    <t>Get the future out of your head</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.314</t>
+  </si>
+  <si>
+    <t>Clarity equals success</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.326</t>
+  </si>
+  <si>
+    <t>Same habits, same results</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.339</t>
+  </si>
+  <si>
+    <t>Changes that seem small and unimportant at first will compound into remarkable results if you are willing to stick with them for years</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.352</t>
+  </si>
+  <si>
+    <t>In the long run, the quality of our lives often depends on the quality of our habits</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.365</t>
+  </si>
+  <si>
+    <t>Mastery requires patience</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.378</t>
+  </si>
+  <si>
+    <t>Goals are good for setting a direction, but systems are best for making progress</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.39</t>
+  </si>
+  <si>
+    <t>True behavior change is identity change</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.401</t>
+  </si>
+  <si>
+    <t>Habits create freedom</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.412</t>
+  </si>
+  <si>
+    <t>Simple is better than complex</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.423</t>
+  </si>
+  <si>
+    <t>Complex is better than complicated</t>
+  </si>
+  <si>
+    <t>2022-02-15 17:59:18.434</t>
+  </si>
+  <si>
     <t>Without great solitude no serious work is possible</t>
   </si>
   <si>
-    <t>2022-02-15 17:59:17.958</t>
+    <t>2022-02-16 00:04:10.79</t>
   </si>
   <si>
     <t>Distinguish the vital few from the trivial many</t>
   </si>
   <si>
-    <t>2022-02-15 17:59:18.02</t>
-  </si>
-  <si>
     <t>Living by design, not by default</t>
   </si>
   <si>
-    <t>2022-02-15 17:59:18.026</t>
-  </si>
-  <si>
     <t>Sometimes what you don't do is just as important as what you do</t>
   </si>
   <si>
-    <t>2022-02-15 17:59:18.032</t>
-  </si>
-  <si>
     <t>Saying yes to any opportunity by definition requires saying no to several others</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.038</t>
-  </si>
-  <si>
-    <t>What do I want to go big on?</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.044</t>
-  </si>
-  <si>
-    <t>The faintest pencil is better than the strongest memory</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.05</t>
-  </si>
-  <si>
-    <t>A little nonsense now and then is cherished by the wisest men</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.055</t>
-  </si>
-  <si>
-    <t>Your health is your greatest wealth</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.061</t>
-  </si>
-  <si>
-    <t>Escape to quiet thinking and boredom</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.067</t>
-  </si>
-  <si>
-    <t>Ultimate focus. Eliminate distractions</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.074</t>
-  </si>
-  <si>
-    <t>Exceptional people are built in solitude</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.08</t>
-  </si>
-  <si>
-    <t>The magic is that there is no magic. Start where you are. Don't stop</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.087</t>
-  </si>
-  <si>
-    <t>Not lack of time, but lack of direction</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.093</t>
-  </si>
-  <si>
-    <t>Be humble, stay hungry</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.1</t>
-  </si>
-  <si>
-    <t>Saying what you mean and meaning what you say</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.108</t>
-  </si>
-  <si>
-    <t>If it isn't a clear yes, then it's a clear no</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.119</t>
-  </si>
-  <si>
-    <t>To follow, without halt, one aim: there is the secret to success</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.127</t>
-  </si>
-  <si>
-    <t>Half of the troubles of this life can be traced to saying yes too quickly and not saying no soon enough</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.135</t>
-  </si>
-  <si>
-    <t>Less but better</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.144</t>
-  </si>
-  <si>
-    <t>The main thing is to keep the main thing the main thing</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.151</t>
-  </si>
-  <si>
-    <t>Comfortable with cutting losses</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.159</t>
-  </si>
-  <si>
-    <t>Stop making casual commitments</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.166</t>
-  </si>
-  <si>
-    <t>Pause before you speak</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.174</t>
-  </si>
-  <si>
-    <t>Get over the fear of missing out</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.181</t>
-  </si>
-  <si>
-    <t>I saw the angel in the marble and carved until I set him free</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.189</t>
-  </si>
-  <si>
-    <t>No is a complete sentence</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.197</t>
-  </si>
-  <si>
-    <t>If you don't set boundaries - there won't be any</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.204</t>
-  </si>
-  <si>
-    <t>Give me 6 hours to chop down a tree and I will spend the first 4 sharpening the axe</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.212</t>
-  </si>
-  <si>
-    <t>The only thing we can expect (with any great certainty) is the unexpected</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.22</t>
-  </si>
-  <si>
-    <t>To attain knowledge add things every day. To attain wisdom subtract things every day</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.228</t>
-  </si>
-  <si>
-    <t>All it takes is a small shove, then momentum will naturally build</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.241</t>
-  </si>
-  <si>
-    <t>Look for small changes you can do in areas you do often. There is power in steadiness and repetition</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.255</t>
-  </si>
-  <si>
-    <t>Done is better than perfect</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.266</t>
-  </si>
-  <si>
-    <t>Routine, in an intelligent man, is a sign of ambition</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.279</t>
-  </si>
-  <si>
-    <t>Routine eliminates nonessential distractions and enshrines the essentials</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.29</t>
-  </si>
-  <si>
-    <t>Do the most difficult thing first</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.302</t>
-  </si>
-  <si>
-    <t>Get the future out of your head</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.314</t>
-  </si>
-  <si>
-    <t>Clarity equals success</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.326</t>
-  </si>
-  <si>
-    <t>Same habits, same results</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.339</t>
-  </si>
-  <si>
-    <t>Changes that seem small and unimportant at first will compound into remarkable results if you are willing to stick with them for years</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.352</t>
-  </si>
-  <si>
-    <t>In the long run, the quality of our lives often depends on the quality of our habits</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.365</t>
-  </si>
-  <si>
-    <t>Mastery requires patience</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.378</t>
-  </si>
-  <si>
-    <t>Goals are good for setting a direction, but systems are best for making progress</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.39</t>
-  </si>
-  <si>
-    <t>True behavior change is identity change</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.401</t>
-  </si>
-  <si>
-    <t>Habits create freedom</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.412</t>
-  </si>
-  <si>
-    <t>Simple is better than complex</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.423</t>
-  </si>
-  <si>
-    <t>Complex is better than complicated</t>
-  </si>
-  <si>
-    <t>2022-02-15 17:59:18.434</t>
   </si>
   <si>
     <t>word</t>
@@ -1185,7 +1195,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1195,395 +1205,35 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" t="s">
-        <v>98</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1592,6 +1242,414 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:G85"/>
   <sheetViews>
@@ -1601,1453 +1659,1453 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D2" t="n">
         <v>1.0</v>
       </c>
       <c r="G2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D3" t="n">
         <v>1.0</v>
       </c>
       <c r="G3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D4" t="n">
         <v>1.0</v>
       </c>
       <c r="G4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D5" t="n">
         <v>0.0</v>
       </c>
       <c r="G5" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D6" t="n">
         <v>1.0</v>
       </c>
       <c r="G6" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D7" t="n">
         <v>1.0</v>
       </c>
       <c r="G7" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D8" t="n">
         <v>1.0</v>
       </c>
       <c r="G8" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D9" t="n">
         <v>0.0</v>
       </c>
       <c r="G9" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D10" t="n">
         <v>1.0</v>
       </c>
       <c r="G10" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D11" t="n">
         <v>1.0</v>
       </c>
       <c r="G11" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D12" t="n">
         <v>1.0</v>
       </c>
       <c r="G12" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D13" t="n">
         <v>1.0</v>
       </c>
       <c r="G13" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D14" t="n">
         <v>1.0</v>
       </c>
       <c r="G14" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B15" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C15" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D15" t="n">
         <v>0.0</v>
       </c>
       <c r="G15" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B16" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C16" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D16" t="n">
         <v>1.0</v>
       </c>
       <c r="G16" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="B17" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C17" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D17" t="n">
         <v>1.0</v>
       </c>
       <c r="G17" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B18" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C18" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D18" t="n">
         <v>1.0</v>
       </c>
       <c r="G18" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C19" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D19" t="n">
         <v>0.0</v>
       </c>
       <c r="G19" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D20" t="n">
         <v>1.0</v>
       </c>
       <c r="G20" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B21" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C21" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="D21" t="n">
         <v>1.0</v>
       </c>
       <c r="G21" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B22" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C22" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D22" t="n">
         <v>1.0</v>
       </c>
       <c r="G22" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D23" t="n">
         <v>1.0</v>
       </c>
       <c r="G23" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C24" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D24" t="n">
         <v>1.0</v>
       </c>
       <c r="G24" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B25" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C25" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="D25" t="n">
         <v>1.0</v>
       </c>
       <c r="G25" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B26" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C26" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D26" t="n">
         <v>0.0</v>
       </c>
       <c r="G26" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B27" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C27" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D27" t="n">
         <v>1.0</v>
       </c>
       <c r="G27" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B28" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C28" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D28" t="n">
         <v>0.0</v>
       </c>
       <c r="G28" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C29" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D29" t="n">
         <v>1.0</v>
       </c>
       <c r="G29" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B30" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C30" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D30" t="n">
         <v>1.0</v>
       </c>
       <c r="G30" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B31" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C31" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D31" t="n">
         <v>0.0</v>
       </c>
       <c r="G31" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B32" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="C32" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D32" t="n">
         <v>1.0</v>
       </c>
       <c r="G32" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D33" t="n">
         <v>1.0</v>
       </c>
       <c r="G33" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C34" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D34" t="n">
         <v>1.0</v>
       </c>
       <c r="G34" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B35" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D35" t="n">
         <v>1.0</v>
       </c>
       <c r="G35" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B36" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C36" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="D36" t="n">
         <v>1.0</v>
       </c>
       <c r="G36" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C37" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D37" t="n">
         <v>1.0</v>
       </c>
       <c r="G37" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="B38" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C38" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D38" t="n">
         <v>1.0</v>
       </c>
       <c r="G38" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D39" t="n">
         <v>0.0</v>
       </c>
       <c r="G39" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B40" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C40" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D40" t="n">
         <v>1.0</v>
       </c>
       <c r="G40" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C41" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D41" t="n">
         <v>0.0</v>
       </c>
       <c r="G41" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B42" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C42" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D42" t="n">
         <v>1.0</v>
       </c>
       <c r="G42" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B43" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D43" t="n">
         <v>0.0</v>
       </c>
       <c r="G43" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B44" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C44" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D44" t="n">
         <v>0.0</v>
       </c>
       <c r="G44" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="B45" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C45" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D45" t="n">
         <v>1.0</v>
       </c>
       <c r="G45" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D46" t="n">
         <v>1.0</v>
       </c>
       <c r="G46" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B47" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C47" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D47" t="n">
         <v>1.0</v>
       </c>
       <c r="G47" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C48" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D48" t="n">
         <v>0.0</v>
       </c>
       <c r="G48" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B49" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C49" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D49" t="n">
         <v>0.0</v>
       </c>
       <c r="G49" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="B50" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C50" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D50" t="n">
         <v>0.0</v>
       </c>
       <c r="G50" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="B51" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C51" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D51" t="n">
         <v>0.0</v>
       </c>
       <c r="G51" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B52" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C52" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D52" t="n">
         <v>0.0</v>
       </c>
       <c r="G52" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C53" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D53" t="n">
         <v>1.0</v>
       </c>
       <c r="G53" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B54" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C54" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D54" t="n">
         <v>0.0</v>
       </c>
       <c r="G54" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B55" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C55" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D55" t="n">
         <v>1.0</v>
       </c>
       <c r="G55" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C56" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D56" t="n">
         <v>1.0</v>
       </c>
       <c r="G56" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B57" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C57" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D57" t="n">
         <v>0.0</v>
       </c>
       <c r="G57" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B58" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C58" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="D58" t="n">
         <v>0.0</v>
       </c>
       <c r="G58" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B59" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C59" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D59" t="n">
         <v>0.0</v>
       </c>
       <c r="G59" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B60" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C60" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D60" t="n">
         <v>1.0</v>
       </c>
       <c r="G60" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B61" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C61" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="D61" t="n">
         <v>1.0</v>
       </c>
       <c r="G61" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B62" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C62" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D62" t="n">
         <v>1.0</v>
       </c>
       <c r="G62" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C63" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D63" t="n">
         <v>1.0</v>
       </c>
       <c r="G63" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B64" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C64" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D64" t="n">
         <v>1.0</v>
       </c>
       <c r="G64" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B65" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C65" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D65" t="n">
         <v>0.0</v>
       </c>
       <c r="G65" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="B66" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C66" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="D66" t="n">
         <v>1.0</v>
       </c>
       <c r="G66" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="B67" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C67" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D67" t="n">
         <v>0.0</v>
       </c>
       <c r="G67" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C68" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="D68" t="n">
         <v>1.0</v>
       </c>
       <c r="G68" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="B69" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C69" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="D69" t="n">
         <v>0.0</v>
       </c>
       <c r="G69" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B70" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C70" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="D70" t="n">
         <v>1.0</v>
       </c>
       <c r="G70" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B71" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C71" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="D71" t="n">
         <v>1.0</v>
       </c>
       <c r="G71" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B72" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C72" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="D72" t="n">
         <v>0.0</v>
       </c>
       <c r="G72" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B73" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C73" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D73" t="n">
         <v>1.0</v>
       </c>
       <c r="G73" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B74" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C74" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="D74" t="n">
         <v>1.0</v>
       </c>
       <c r="G74" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B75" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C75" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="D75" t="n">
         <v>1.0</v>
       </c>
       <c r="G75" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B76" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C76" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="D76" t="n">
         <v>1.0</v>
       </c>
       <c r="G76" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="B77" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C77" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="D77" t="n">
         <v>1.0</v>
       </c>
       <c r="G77" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="B78" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C78" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D78" t="n">
         <v>0.0</v>
       </c>
       <c r="G78" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B79" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C79" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="D79" t="n">
         <v>1.0</v>
       </c>
       <c r="G79" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B80" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C80" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="D80" t="n">
         <v>1.0</v>
       </c>
       <c r="G80" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="B81" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C81" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="D81" t="n">
         <v>2.0</v>
       </c>
       <c r="G81" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B82" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C82" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D82" t="n">
         <v>2.0</v>
       </c>
       <c r="G82" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="B83" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C83" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="D83" t="n">
         <v>1.0</v>
       </c>
       <c r="G83" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="B84" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C84" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="D84" t="n">
         <v>1.0</v>
       </c>
       <c r="G84" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B85" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C85" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="D85" t="n">
         <v>1.0</v>
       </c>
       <c r="G85" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: (upload-service) upload settings
</commit_message>
<xml_diff>
--- a/upload.xlsx
+++ b/upload.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tags" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="notes" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="ENGLISH" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="English" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="settings" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="383">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -1162,6 +1163,15 @@
   </si>
   <si>
     <t xml:space="preserve">2022-02-15 17:59:21.504</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default language name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entries per vocabulary training session</t>
+  </si>
+  <si>
+    <t xml:space="preserve">English</t>
   </si>
 </sst>
 </file>
@@ -1176,6 +1186,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1235,8 +1246,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1263,45 +1278,45 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1323,447 +1338,447 @@
   </sheetPr>
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="125.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="125.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.04"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="0" t="s">
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="0" t="s">
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="0" t="s">
+      <c r="B19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>99</v>
       </c>
     </row>
@@ -1789,1261 +1804,1261 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="0" t="s">
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="0" t="s">
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="0" t="s">
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="0" t="s">
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="0" t="s">
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="0" t="s">
+      <c r="D8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="0" t="s">
+      <c r="D10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="0" t="s">
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="0" t="s">
+      <c r="D12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="0" t="s">
+      <c r="D13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="0" t="s">
+      <c r="D14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="1" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="0" t="s">
+      <c r="D16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="0" t="s">
+      <c r="D17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G18" s="0" t="s">
+      <c r="D18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D20" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G20" s="0" t="s">
+      <c r="D20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="0" t="s">
+      <c r="D21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G22" s="0" t="s">
+      <c r="D22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G23" s="0" t="s">
+      <c r="D23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G24" s="0" t="s">
+      <c r="D24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G25" s="0" t="s">
+      <c r="D25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="0" t="s">
+      <c r="G26" s="1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G27" s="0" t="s">
+      <c r="D27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="0" t="s">
+      <c r="G28" s="1" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G29" s="0" t="s">
+      <c r="D29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G30" s="0" t="s">
+      <c r="D30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="0" t="s">
+      <c r="G31" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G32" s="0" t="s">
+      <c r="D32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G33" s="0" t="s">
+      <c r="D33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D34" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G34" s="0" t="s">
+      <c r="D34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D35" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G35" s="0" t="s">
+      <c r="D35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D36" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G36" s="0" t="s">
+      <c r="D36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G37" s="0" t="s">
+      <c r="D37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D38" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G38" s="0" t="s">
+      <c r="D38" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G39" s="0" t="s">
+      <c r="G39" s="1" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D40" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G40" s="0" t="s">
+      <c r="D40" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" s="1" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="D41" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G41" s="0" t="s">
+      <c r="G41" s="1" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D42" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G42" s="0" t="s">
+      <c r="D42" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G43" s="0" t="s">
+      <c r="G43" s="1" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="D44" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G44" s="0" t="s">
+      <c r="G44" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G45" s="0" t="s">
+      <c r="D45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="D46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G46" s="0" t="s">
+      <c r="D46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G47" s="0" t="s">
+      <c r="D47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D48" s="0" t="n">
+      <c r="D48" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G48" s="0" t="s">
+      <c r="G48" s="1" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D49" s="0" t="n">
+      <c r="D49" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G49" s="0" t="s">
+      <c r="G49" s="1" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="D50" s="0" t="n">
+      <c r="D50" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G50" s="0" t="s">
+      <c r="G50" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="D51" s="0" t="n">
+      <c r="D51" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G51" s="0" t="s">
+      <c r="G51" s="1" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D52" s="0" t="n">
+      <c r="D52" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G52" s="0" t="s">
+      <c r="G52" s="1" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="D53" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G53" s="0" t="s">
+      <c r="D53" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="D54" s="0" t="n">
+      <c r="D54" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G54" s="0" t="s">
+      <c r="G54" s="1" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="D55" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G55" s="0" t="s">
+      <c r="D55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="D56" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G56" s="0" t="s">
+      <c r="D56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" s="1" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="D57" s="0" t="n">
+      <c r="D57" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G57" s="0" t="s">
+      <c r="G57" s="1" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="D58" s="0" t="n">
+      <c r="D58" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G58" s="0" t="s">
+      <c r="G58" s="1" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="D59" s="0" t="n">
+      <c r="D59" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G59" s="0" t="s">
+      <c r="G59" s="1" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D60" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="0" t="s">
+      <c r="D60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="D61" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G61" s="0" t="s">
+      <c r="D61" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="D62" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G62" s="0" t="s">
+      <c r="D62" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="D63" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G63" s="0" t="s">
+      <c r="D63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="D64" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G64" s="0" t="s">
+      <c r="D64" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="D65" s="0" t="n">
+      <c r="D65" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G65" s="0" t="s">
+      <c r="G65" s="1" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D66" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G66" s="0" t="s">
+      <c r="D66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D67" s="0" t="n">
+      <c r="D67" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G67" s="0" t="s">
+      <c r="G67" s="1" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="D68" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G68" s="0" t="s">
+      <c r="D68" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C69" s="0" t="s">
+      <c r="C69" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="D69" s="0" t="n">
+      <c r="D69" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G69" s="0" t="s">
+      <c r="G69" s="1" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="C70" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="D70" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G70" s="0" t="s">
+      <c r="D70" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G70" s="1" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C71" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="D71" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G71" s="0" t="s">
+      <c r="D71" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="D72" s="0" t="n">
+      <c r="D72" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G72" s="0" t="s">
+      <c r="G72" s="1" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C73" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="D73" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G73" s="0" t="s">
+      <c r="D73" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G73" s="1" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="C74" s="0" t="s">
+      <c r="C74" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="D74" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G74" s="0" t="s">
+      <c r="D74" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G74" s="1" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="C75" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="D75" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G75" s="0" t="s">
+      <c r="D75" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G75" s="1" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C76" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="D76" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G76" s="0" t="s">
+      <c r="D76" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="C77" s="0" t="s">
+      <c r="C77" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="D77" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G77" s="0" t="s">
+      <c r="D77" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" s="1" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="D78" s="0" t="n">
+      <c r="D78" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G78" s="0" t="s">
+      <c r="G78" s="1" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="C79" s="0" t="s">
+      <c r="C79" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="D79" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G79" s="0" t="s">
+      <c r="D79" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="C80" s="0" t="s">
+      <c r="C80" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="D80" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G80" s="0" t="s">
+      <c r="D80" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G80" s="1" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C81" s="0" t="s">
+      <c r="C81" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="D81" s="0" t="n">
+      <c r="D81" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G81" s="0" t="s">
+      <c r="G81" s="1" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="C82" s="0" t="s">
+      <c r="C82" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="D82" s="0" t="n">
+      <c r="D82" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G82" s="0" t="s">
+      <c r="G82" s="1" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="C83" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="D83" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G83" s="0" t="s">
+      <c r="D83" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="C84" s="0" t="s">
+      <c r="C84" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D84" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G84" s="0" t="s">
+      <c r="D84" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G84" s="1" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="C85" s="0" t="s">
+      <c r="C85" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="D85" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G85" s="0" t="s">
+      <c r="D85" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G85" s="1" t="s">
         <v>379</v>
       </c>
     </row>
@@ -3056,4 +3071,48 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.54"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: (upload-service) remove hardcoded sheet names
</commit_message>
<xml_diff>
--- a/upload.xlsx
+++ b/upload.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tags" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="notes" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="English" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="language_English" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="settings" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -1278,7 +1278,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1342,7 +1342,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="125.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.04"/>
@@ -1800,11 +1800,11 @@
   </sheetPr>
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3080,13 +3080,13 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.54"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
feat: (upload-service) upload/download settings with pagination parameters
</commit_message>
<xml_diff>
--- a/upload.xlsx
+++ b/upload.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tags" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="387">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -1169,6 +1169,18 @@
   </si>
   <si>
     <t xml:space="preserve">entries per vocabulary training session</t>
+  </si>
+  <si>
+    <t xml:space="preserve">languages pagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags pagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes pagination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vocabulary pagination</t>
   </si>
   <si>
     <t xml:space="preserve">English</t>
@@ -1278,7 +1290,7 @@
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1342,7 +1354,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="125.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.04"/>
@@ -1800,11 +1812,11 @@
   </sheetPr>
   <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3078,16 +3090,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.81"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3097,13 +3113,37 @@
       <c r="B1" s="0" t="s">
         <v>381</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>6</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>